<commit_message>
acrescenta círculo maior no último valor da série. ajusta textos dos eixos para aumentar seu tamanho (alterei ordem de grandeza e precisão dos valores nos eixos). atualiza RData e tabela PAF.
</commit_message>
<xml_diff>
--- a/modulo-grandes-numeros/grandes-numeros/dados_PAF.xlsx
+++ b/modulo-grandes-numeros/grandes-numeros/dados_PAF.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago.pereira\Documents\GitHub\projeto-divida\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago.pereira\Documents\GitHub\projeto-divida\modulo-grandes-numeros\grandes-numeros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E21A0880-A54F-4100-8369-00038917E6A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E64CD4-9D66-4B15-9EE7-9CB76BC64D05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" xr2:uid="{92102A9E-DF42-444A-802B-A651F0B77722}"/>
   </bookViews>
@@ -443,7 +443,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -477,10 +477,10 @@
         <v>3</v>
       </c>
       <c r="C2" s="2">
-        <v>4100</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D2" s="2">
-        <v>4300</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>